<commit_message>
Changed the Domain Community of OIOUBL doc types; TICC-402
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.3.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/dev/git-peppol/edec-codelists/work-in-progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA7B5C2-F9D0-7F40-ABD0-10BF4803A84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265E8316-9439-B645-9B62-BDEE865D4800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3333,8 +3333,8 @@
   <dimension ref="A1:N307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A306" sqref="A306"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5235,7 +5235,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>111</v>
+        <v>578</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>696</v>
@@ -5271,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>111</v>
+        <v>578</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>697</v>

</xml_diff>